<commit_message>
error message is now displayed if error occures and debugging
An error window was created along with an error window function. The error window functions gets called if an error occures in the execution which opens a top level window with the error description. Main errors have custom messages, other errors display the python error message directly.

Some bugs were fixed too:
- There is no problem now if a liquidaciones input contains no items, no items without CSG column or no items with CSG column.
- BarraBusqueda class got an update: the text inside the text widget within the class now desapears and reapears as expected.
</commit_message>
<xml_diff>
--- a/data/output/program_output/control.xlsx
+++ b/data/output/program_output/control.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="202">
   <si>
     <t>2022-W1</t>
   </si>
@@ -2185,51 +2185,6 @@
       <c r="BG6" t="s">
         <v>123</v>
       </c>
-      <c r="BH6" t="s">
-        <v>126</v>
-      </c>
-      <c r="BI6">
-        <v>400</v>
-      </c>
-      <c r="BJ6">
-        <v>290</v>
-      </c>
-      <c r="BK6">
-        <v>81200</v>
-      </c>
-      <c r="BL6">
-        <v>11768.12</v>
-      </c>
-      <c r="BM6">
-        <v>18.93</v>
-      </c>
-      <c r="BN6">
-        <v>5299.83</v>
-      </c>
-      <c r="BO6">
-        <v>24838.16</v>
-      </c>
-      <c r="BP6">
-        <v>62.09540000000001</v>
-      </c>
-      <c r="BQ6">
-        <v>6.209540000000001</v>
-      </c>
-      <c r="BR6">
-        <v>941.4496</v>
-      </c>
-      <c r="BS6">
-        <v>2.353624</v>
-      </c>
-      <c r="BT6">
-        <v>0.2353624</v>
-      </c>
-      <c r="BU6">
-        <v>25779.6096</v>
-      </c>
-      <c r="BV6">
-        <v>-14011.4896</v>
-      </c>
     </row>
     <row r="7" spans="1:74">
       <c r="A7" t="s">
@@ -2372,51 +2327,6 @@
       </c>
       <c r="BG7" t="s">
         <v>124</v>
-      </c>
-      <c r="BH7" t="s">
-        <v>126</v>
-      </c>
-      <c r="BI7">
-        <v>500</v>
-      </c>
-      <c r="BJ7">
-        <v>290</v>
-      </c>
-      <c r="BK7">
-        <v>24940</v>
-      </c>
-      <c r="BL7">
-        <v>3614.49</v>
-      </c>
-      <c r="BM7">
-        <v>18.93</v>
-      </c>
-      <c r="BN7">
-        <v>1627.81</v>
-      </c>
-      <c r="BO7">
-        <v>31047.7</v>
-      </c>
-      <c r="BP7">
-        <v>62.0954</v>
-      </c>
-      <c r="BQ7">
-        <v>6.209540000000001</v>
-      </c>
-      <c r="BR7">
-        <v>289.1592</v>
-      </c>
-      <c r="BS7">
-        <v>0.5783184</v>
-      </c>
-      <c r="BT7">
-        <v>0.05783184</v>
-      </c>
-      <c r="BU7">
-        <v>31336.8592</v>
-      </c>
-      <c r="BV7">
-        <v>-27722.3692</v>
       </c>
     </row>
   </sheetData>

</xml_diff>